<commit_message>
atualiza divisão de telas e insere planilhas de relatórios
</commit_message>
<xml_diff>
--- a/docs_organizados/Outros/Divisão_Telas.xlsx
+++ b/docs_organizados/Outros/Divisão_Telas.xlsx
@@ -662,7 +662,7 @@
   <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -949,7 +949,7 @@
       <c r="C26" s="15"/>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="18"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="17" t="s">
@@ -959,7 +959,7 @@
       <c r="C27" s="15"/>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
-      <c r="F27" s="18"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="17" t="s">
@@ -969,7 +969,7 @@
       <c r="C28" s="15"/>
       <c r="D28" s="15"/>
       <c r="E28" s="15"/>
-      <c r="F28" s="18"/>
+      <c r="F28" s="9"/>
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="17" t="s">
@@ -979,7 +979,7 @@
       <c r="C29" s="15"/>
       <c r="D29" s="15"/>
       <c r="E29" s="15"/>
-      <c r="F29" s="18"/>
+      <c r="F29" s="9"/>
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="17" t="s">
@@ -989,7 +989,7 @@
       <c r="C30" s="15"/>
       <c r="D30" s="15"/>
       <c r="E30" s="15"/>
-      <c r="F30" s="18"/>
+      <c r="F30" s="9"/>
     </row>
     <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="17" t="s">
@@ -999,7 +999,7 @@
       <c r="C31" s="15"/>
       <c r="D31" s="15"/>
       <c r="E31" s="15"/>
-      <c r="F31" s="18"/>
+      <c r="F31" s="9"/>
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="s">

</xml_diff>